<commit_message>
Add description for publishing.
</commit_message>
<xml_diff>
--- a/3402 Ass2.xlsx
+++ b/3402 Ass2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\16567\Documents\GitHub\2023_SP51_CMS_GroupB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF0947ED-29A5-42EB-B909-A760DDB0D15E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B2AE5AB-9673-4E4E-A8A8-8FFC473ABE2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks Description" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="63">
   <si>
     <t>Theme</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -341,6 +341,18 @@
   </si>
   <si>
     <t>Due Date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Create a production site</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Create a staging site</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>One person in charge of</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -815,8 +827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B5:I64"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1079,24 +1091,62 @@
         <v>47</v>
       </c>
     </row>
+    <row r="44" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="F44" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="G45" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="46" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="G46" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="47" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E47" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F47" s="1"/>
+    </row>
+    <row r="48" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="F48" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="49" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="G49" t="s">
+        <v>35</v>
+      </c>
+      <c r="I49" t="s">
+        <v>34</v>
+      </c>
+    </row>
     <row r="50" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E50" t="s">
-        <v>7</v>
-      </c>
-      <c r="F50" s="3" t="s">
-        <v>18</v>
+      <c r="F50" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="51" spans="5:9" x14ac:dyDescent="0.3">
       <c r="G51" t="s">
-        <v>35</v>
-      </c>
-      <c r="I51" t="s">
-        <v>34</v>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="G52" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="53" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E53" t="s">
+      <c r="G53" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="54" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E54" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1136,7 +1186,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7794AFC9-B11D-479E-A43F-08D6EC184311}">
   <dimension ref="B2:T38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add theme design information based on the content client provided
</commit_message>
<xml_diff>
--- a/3402 Ass2.xlsx
+++ b/3402 Ass2.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\16567\Documents\GitHub\2023_SP51_CMS_GroupB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19CD33D4-356E-4FE1-9C9C-256BC7762B57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63822F74-9D13-43A4-90E3-224067C6FA89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10260" yWindow="2260" windowWidth="14190" windowHeight="11650" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks Description" sheetId="1" r:id="rId1"/>
     <sheet name="Gantt Chart" sheetId="2" r:id="rId2"/>
+    <sheet name="Design Info" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="161">
   <si>
     <t>Theme</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -355,12 +356,418 @@
     <t>One person in charge of</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>specialize in Math and Science from Primary to Junior College</t>
+  </si>
+  <si>
+    <t>Bookings are essential. Could I please suggest that you make your booking as soon as possible so that you will not be disappointed?</t>
+  </si>
+  <si>
+    <t>Please contact us on the Center’s email or BaizonnLearning@gmail.com</t>
+  </si>
+  <si>
+    <t>Or Phone Lum on +65 62811816</t>
+  </si>
+  <si>
+    <t>Address: 1007A Upper Serangoon Road</t>
+  </si>
+  <si>
+    <t>Christmas buffet dinner will be arranged for all guests. Vegetarian menu is available too. Kindly indicate your preference during booking.</t>
+  </si>
+  <si>
+    <t>Unique Baizonn T-Shirt will be given free for all confirmed students during the Open House.</t>
+  </si>
+  <si>
+    <t>Home Tab:</t>
+  </si>
+  <si>
+    <t>Welcome to BAIZONN</t>
+  </si>
+  <si>
+    <t>Founded in 2018, we believe in Establishing a Strong Foundation build on Grasping Maths and Science Principles.</t>
+  </si>
+  <si>
+    <t>At Baizonn, we Equip your child to ace the semester. We provide up-to-date curriculum and targeted lesson to set your child up for success in the coming terms.</t>
+  </si>
+  <si>
+    <t>F.A.S.T. = Firm Foundation, Apply, Surpass, Top</t>
+  </si>
+  <si>
+    <t>S.T.E.M : Science, Technology, Engineering, Maths</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Goals</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Increase students' enrolment</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Target Audience</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Parents + high-school studnets.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Site</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: learning center "BaizonnLearningCenter" </t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NOTE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WordPress posts:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Current sessions</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Promotions</t>
+  </si>
+  <si>
+    <t>Promotions</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Staff details</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WordPress pages:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>About us…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dynamic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Event:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name: Open House for 2023 Intake</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Date: 23rd December 2022, Friday 3pm to 9pm.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Static - not change frequently, not author, data, tag…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>etc. (events)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>General Inquiries: 62811816, or BaizonnLearning@gmail.com</t>
+  </si>
+  <si>
+    <t>Contatct Details:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A center image -- Named: Centre Logo 9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nurturing a Love For Learning</t>
+  </si>
+  <si>
+    <t>For over 5 years, we help students achieve success in school and in life by nurturing a love for learning.</t>
+  </si>
+  <si>
+    <t>From primary school to junior college, our students enjoy fun, interactive and relevant lessons and are empowered to think beyond the confines of the classroom.</t>
+  </si>
+  <si>
+    <t>Preparing Students To Achieve Success</t>
+  </si>
+  <si>
+    <t>Developing Confident and Successful Learners</t>
+  </si>
+  <si>
+    <t>Our students are at the centre of everything we do and their well-being and success in learning matter to us.</t>
+  </si>
+  <si>
+    <t>While we educate our students, we also equip them with the right knowledge, skills and attitudes that help them solve problems, think big and seek excellence.</t>
+  </si>
+  <si>
+    <t>Passionate Teachers That Make A Difference</t>
+  </si>
+  <si>
+    <t>Our teachers motivate and nurture every student to achieve their best and to build the right attitudes to ingrain a love for learning.</t>
+  </si>
+  <si>
+    <t>We hire teachers with the right passion and qualifications, and equip them to create amazing classroom experiences for their students.</t>
+  </si>
+  <si>
+    <t>We're committed to bringing out the best in every student.</t>
+  </si>
+  <si>
+    <t>About Us Tab:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Registration Tab:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Join Us at Baizonn!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>And a contact form</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name*</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Contact Number*</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Email*</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Your school</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Your grade</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Message</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Class interested</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Schedule Tab:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Filter -- All classes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A timetable like the one in student first</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Other Resources:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Subjects offer</t>
+  </si>
+  <si>
+    <t>Science</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Secondary 1-2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Secondary 3-4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Junior College 1-2 </t>
+  </si>
+  <si>
+    <t>Mathematics</t>
+  </si>
+  <si>
+    <t>Primary 3-6</t>
+  </si>
+  <si>
+    <t>Junior College 1-2</t>
+  </si>
+  <si>
+    <t>Advanced Courses</t>
+  </si>
+  <si>
+    <t>Integrated Programme (IP) Mathematics and Science</t>
+  </si>
+  <si>
+    <t>International Baccalaureate (IB) Mathematics and Science</t>
+  </si>
+  <si>
+    <t>Science</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Academic Partner</t>
+  </si>
+  <si>
+    <t>Academic Channel Partner for S.T.E.M.</t>
+  </si>
+  <si>
+    <t>NATIONAL INSTRUMENTS -- we have its logo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Primary 3-6 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Primary Science</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Secondary 1-2 Science</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Secondary 3-4 Physics, Chemistry and Biology</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Junior College H1, H2 Physics, Chemistry and Biology</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Primary Mathematics</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Seconday 1-2 Mathematics</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Seconday 3-4 Elementary Mathematics, Additional Mathematics</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Junior College H1, H2, H3 Mathematics</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Awards</t>
+  </si>
+  <si>
+    <t>“A Smart Recirculating Aquaculture System”</t>
+  </si>
+  <si>
+    <t>Winner of Editor’s Choice Awards for 2016 Engineering Impact Awards ASEAN / ANZ Regional Contest</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total Four awards images -- see the content given</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Current Session for 2022</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>View the A01 Center Info word document or the image in Discord</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Include the time and monthly fee</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>For students that enrolled into 2 subjects, there will be 5% discount on the monthly fees.</t>
+  </si>
+  <si>
+    <t>For students that enrolled into 3 subjects, there will be 10% discount on the monthly fees</t>
+  </si>
+  <si>
+    <t>Video</t>
+  </si>
+  <si>
+    <t>Basics Algebra for Beginners</t>
+  </si>
+  <si>
+    <t>38 mins</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=PVoTRu3p6ug</t>
+  </si>
+  <si>
+    <t>12 mins</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=kWOTmyoaWJg</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -434,6 +841,25 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -500,7 +926,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -554,6 +980,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -836,7 +1265,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:I64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -1650,4 +2079,530 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EAC2AC4-0C1C-43C2-BF40-AC3F49B518A9}">
+  <dimension ref="B3:J130"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D125" sqref="D125"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B3" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B6" s="10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B7" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="J7" s="24"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B9" s="27" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D17" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D18" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B20" s="27" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D24" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D27" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D29" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D30" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B32" s="27" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C33" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C34" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B51" s="27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C52" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C54" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C55" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C57" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C58" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B60" s="27" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C61" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C62" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D63" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D64" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C66" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D67" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D68" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D69" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C70" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D71" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D72" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D73" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B75" s="27" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C76" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C77" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D78" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D79" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="80" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D80" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="81" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D81" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="82" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D82" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="83" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D83" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="84" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D84" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="86" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B86" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="87" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C87" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="88" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C88" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="90" spans="2:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B90" s="28" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="91" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C91" s="29" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="92" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D92" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="93" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D93" t="s">
+        <v>137</v>
+      </c>
+      <c r="G93" t="s">
+        <v>123</v>
+      </c>
+      <c r="I93" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="94" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D94" t="s">
+        <v>124</v>
+      </c>
+      <c r="G94" t="s">
+        <v>133</v>
+      </c>
+      <c r="I94" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="95" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D95" t="s">
+        <v>125</v>
+      </c>
+      <c r="G95" t="s">
+        <v>123</v>
+      </c>
+      <c r="I95" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="96" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D96" t="s">
+        <v>126</v>
+      </c>
+      <c r="G96" t="s">
+        <v>123</v>
+      </c>
+      <c r="I96" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="98" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="D98" s="24" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="99" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="D99" t="s">
+        <v>128</v>
+      </c>
+      <c r="G99" t="s">
+        <v>127</v>
+      </c>
+      <c r="I99" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="100" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="D100" t="s">
+        <v>124</v>
+      </c>
+      <c r="G100" t="s">
+        <v>127</v>
+      </c>
+      <c r="I100" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="101" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="D101" t="s">
+        <v>125</v>
+      </c>
+      <c r="G101" t="s">
+        <v>127</v>
+      </c>
+      <c r="I101" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="102" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="D102" t="s">
+        <v>129</v>
+      </c>
+      <c r="G102" t="s">
+        <v>127</v>
+      </c>
+      <c r="I102" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="104" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="D104" s="24" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="105" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="D105" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="106" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="D106" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="108" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C108" s="29" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="109" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="D109" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="110" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="D110" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="112" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C112" s="29" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="113" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D113" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="114" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D114" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="115" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D115" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="117" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C117" s="29" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="118" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D118" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="119" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D119" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="121" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C121" s="29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="122" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D122" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="123" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D123" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="125" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C125" s="29" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="126" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D126" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="127" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D127" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="128" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D128" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="129" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D129" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="130" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D130" t="s">
+        <v>160</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update design information from the images the client provides
</commit_message>
<xml_diff>
--- a/3402 Ass2.xlsx
+++ b/3402 Ass2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\16567\Documents\GitHub\2023_SP51_CMS_GroupB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63822F74-9D13-43A4-90E3-224067C6FA89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7CA5EC5-CCAD-4083-8073-28FF599E5C4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10260" yWindow="2260" windowWidth="14190" windowHeight="11650" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3800" yWindow="5270" windowWidth="14190" windowHeight="11650" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks Description" sheetId="1" r:id="rId1"/>
@@ -390,9 +390,6 @@
     <t>At Baizonn, we Equip your child to ace the semester. We provide up-to-date curriculum and targeted lesson to set your child up for success in the coming terms.</t>
   </si>
   <si>
-    <t>F.A.S.T. = Firm Foundation, Apply, Surpass, Top</t>
-  </si>
-  <si>
     <t>S.T.E.M : Science, Technology, Engineering, Maths</t>
   </si>
   <si>
@@ -630,9 +627,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Subjects offer</t>
-  </si>
-  <si>
     <t>Science</t>
   </si>
   <si>
@@ -761,6 +755,14 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=kWOTmyoaWJg</t>
+  </si>
+  <si>
+    <t>F.A.S.T. = Firm Foundation, Apply, Surpass, Top (Note for the image in the content)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Subjects offer (Note for the image in the content)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2083,17 +2085,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EAC2AC4-0C1C-43C2-BF40-AC3F49B518A9}">
-  <dimension ref="B3:J130"/>
+  <dimension ref="B3:J115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D125" sqref="D125"/>
+    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B3" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.3">
@@ -2103,78 +2105,78 @@
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B6" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J7" s="24"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" s="27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="D14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="D15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" s="27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.3">
@@ -2209,47 +2211,112 @@
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B32" s="27" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C33" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C34" t="s">
-        <v>93</v>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B36" s="27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C37" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C39" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C40" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C42" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C43" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B45" s="27" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C46" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C47" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D48" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D49" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B51" s="27" t="s">
-        <v>70</v>
+      <c r="C51" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C52" t="s">
-        <v>71</v>
+      <c r="D52" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D53" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C54" t="s">
-        <v>72</v>
+      <c r="D54" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C55" t="s">
-        <v>73</v>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D56" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C57" t="s">
-        <v>74</v>
+      <c r="D57" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C58" t="s">
-        <v>75</v>
+      <c r="D58" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.3">
@@ -2259,345 +2326,280 @@
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C61" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C62" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D63" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D64" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C66" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="65" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D65" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="66" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D66" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="67" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D67" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="68" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D68" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="69" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D69" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C70" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D71" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D72" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D73" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B75" s="27" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C76" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C77" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="71" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B71" s="27" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="72" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C72" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="73" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C73" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="75" spans="2:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B75" s="28" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="76" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C76" s="29" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="77" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D77" s="24" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="78" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D78" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="79" spans="2:4" x14ac:dyDescent="0.3">
+        <v>135</v>
+      </c>
+      <c r="G78" t="s">
+        <v>121</v>
+      </c>
+      <c r="I78" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="79" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D79" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+      <c r="G79" t="s">
+        <v>131</v>
+      </c>
+      <c r="I79" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="80" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D80" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="81" spans="2:9" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+      <c r="G80" t="s">
+        <v>121</v>
+      </c>
+      <c r="I80" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="81" spans="3:9" x14ac:dyDescent="0.3">
       <c r="D81" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="82" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D82" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="83" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D83" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="84" spans="2:9" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+      <c r="G81" t="s">
+        <v>121</v>
+      </c>
+      <c r="I81" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="83" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="D83" s="24" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="84" spans="3:9" x14ac:dyDescent="0.3">
       <c r="D84" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="86" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B86" s="27" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="87" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C87" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="88" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C88" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="90" spans="2:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B90" s="28" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="91" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C91" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="G84" t="s">
+        <v>125</v>
+      </c>
+      <c r="I84" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="85" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="D85" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="92" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D92" s="24" t="s">
+      <c r="G85" t="s">
+        <v>125</v>
+      </c>
+      <c r="I85" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="86" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="D86" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="93" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D93" t="s">
-        <v>137</v>
-      </c>
-      <c r="G93" t="s">
-        <v>123</v>
-      </c>
-      <c r="I93" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="94" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="G86" t="s">
+        <v>125</v>
+      </c>
+      <c r="I86" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="87" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="D87" t="s">
+        <v>127</v>
+      </c>
+      <c r="G87" t="s">
+        <v>125</v>
+      </c>
+      <c r="I87" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="89" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="D89" s="24" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="90" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="D90" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="91" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="D91" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="93" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C93" s="29" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="94" spans="3:9" x14ac:dyDescent="0.3">
       <c r="D94" t="s">
-        <v>124</v>
-      </c>
-      <c r="G94" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="95" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="D95" t="s">
         <v>133</v>
       </c>
-      <c r="I94" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="95" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D95" t="s">
-        <v>125</v>
-      </c>
-      <c r="G95" t="s">
-        <v>123</v>
-      </c>
-      <c r="I95" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="96" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D96" t="s">
-        <v>126</v>
-      </c>
-      <c r="G96" t="s">
-        <v>123</v>
-      </c>
-      <c r="I96" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="98" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="D98" s="24" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="99" spans="3:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="97" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C97" s="29" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="98" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D98" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="99" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D99" t="s">
-        <v>128</v>
-      </c>
-      <c r="G99" t="s">
-        <v>127</v>
-      </c>
-      <c r="I99" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="100" spans="3:9" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="100" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D100" t="s">
-        <v>124</v>
-      </c>
-      <c r="G100" t="s">
-        <v>127</v>
-      </c>
-      <c r="I100" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="101" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="D101" t="s">
-        <v>125</v>
-      </c>
-      <c r="G101" t="s">
-        <v>127</v>
-      </c>
-      <c r="I101" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="102" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="D102" t="s">
-        <v>129</v>
-      </c>
-      <c r="G102" t="s">
-        <v>127</v>
-      </c>
-      <c r="I102" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="104" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="D104" s="24" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="105" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="D105" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="106" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="D106" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="108" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C108" s="29" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="109" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="D109" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="110" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="D110" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="112" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C112" s="29" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="113" spans="3:4" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="102" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C102" s="29" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="103" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D103" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="104" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D104" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="106" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C106" s="29" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="107" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D107" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="108" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D108" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="110" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C110" s="29" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="111" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D111" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="112" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D112" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="113" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D113" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="114" spans="3:4" x14ac:dyDescent="0.3">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="114" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D114" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="115" spans="3:4" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="115" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D115" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="117" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C117" s="29" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="118" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="D118" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="119" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="D119" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="121" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C121" s="29" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="122" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="D122" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="123" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="D123" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="125" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C125" s="29" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="126" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="D126" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="127" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="D127" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="128" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="D128" t="s">
         <v>158</v>
-      </c>
-    </row>
-    <row r="129" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D129" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="130" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D130" t="s">
-        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Format the design information
</commit_message>
<xml_diff>
--- a/3402 Ass2.xlsx
+++ b/3402 Ass2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\16567\Documents\GitHub\2023_SP51_CMS_GroupB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7CA5EC5-CCAD-4083-8073-28FF599E5C4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A1A8961-2829-457D-8684-3BB684B878CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3800" yWindow="5270" windowWidth="14190" windowHeight="11650" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3040" yWindow="2750" windowWidth="14190" windowHeight="11650" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks Description" sheetId="1" r:id="rId1"/>
@@ -2085,520 +2085,520 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EAC2AC4-0C1C-43C2-BF40-AC3F49B518A9}">
-  <dimension ref="B3:J115"/>
+  <dimension ref="B2:J113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B2" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B3" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C4" t="s">
+      <c r="C3" t="s">
         <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B5" s="10" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B6" s="10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B7" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="J7" s="24"/>
+      <c r="J6" s="24"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B8" s="27" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B9" s="27" t="s">
-        <v>78</v>
+      <c r="C9" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C10" t="s">
-        <v>79</v>
+      <c r="D10" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="D14" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="D15" t="s">
-        <v>86</v>
+      <c r="C15" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C16" t="s">
-        <v>84</v>
+      <c r="D16" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D17" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D18" t="s">
         <v>90</v>
       </c>
     </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B19" s="27" t="s">
+        <v>87</v>
+      </c>
+    </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B20" s="27" t="s">
-        <v>87</v>
+      <c r="C20" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C21" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
-        <v>89</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D24" t="s">
+      <c r="D23" t="s">
         <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D25" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D26" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D27" t="s">
         <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D28" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D29" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D30" t="s">
         <v>69</v>
       </c>
     </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B31" s="27" t="s">
+        <v>93</v>
+      </c>
+    </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B32" s="27" t="s">
-        <v>93</v>
+      <c r="C32" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C33" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C34" t="s">
         <v>92</v>
       </c>
     </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B35" s="27" t="s">
+        <v>70</v>
+      </c>
+    </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B36" s="27" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C37" t="s">
+      <c r="C36" t="s">
         <v>71</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C38" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C39" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C40" t="s">
         <v>73</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C41" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C42" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C43" t="s">
         <v>74</v>
       </c>
     </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B44" s="27" t="s">
+        <v>106</v>
+      </c>
+    </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B45" s="27" t="s">
-        <v>106</v>
+      <c r="C45" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C46" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C47" t="s">
-        <v>95</v>
+      <c r="D47" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D48" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D49" t="s">
-        <v>97</v>
+      <c r="C49" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D50" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C51" t="s">
-        <v>98</v>
+      <c r="D51" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D52" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D53" t="s">
-        <v>100</v>
+      <c r="C53" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D54" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C55" t="s">
-        <v>102</v>
+      <c r="D55" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D56" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D57" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D58" t="s">
-        <v>105</v>
+      <c r="B58" s="27" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C59" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B60" s="27" t="s">
-        <v>107</v>
+      <c r="C60" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C61" t="s">
-        <v>108</v>
+      <c r="D61" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C62" t="s">
-        <v>109</v>
+      <c r="D62" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D63" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D64" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="65" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D65" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="66" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D66" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="67" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D67" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D68" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="69" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D69" t="s">
-        <v>115</v>
+      <c r="B69" s="27" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="70" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C70" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="71" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B71" s="27" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C72" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C73" t="s">
+      <c r="C71" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="75" spans="2:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B75" s="28" t="s">
+    <row r="73" spans="2:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B73" s="28" t="s">
         <v>120</v>
       </c>
     </row>
+    <row r="74" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C74" s="29" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="75" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D75" s="24" t="s">
+        <v>121</v>
+      </c>
+    </row>
     <row r="76" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C76" s="29" t="s">
-        <v>160</v>
+      <c r="D76" t="s">
+        <v>135</v>
+      </c>
+      <c r="G76" t="s">
+        <v>121</v>
+      </c>
+      <c r="I76" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="77" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D77" s="24" t="s">
-        <v>121</v>
+      <c r="D77" t="s">
+        <v>122</v>
+      </c>
+      <c r="G77" t="s">
+        <v>131</v>
+      </c>
+      <c r="I77" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="78" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D78" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="G78" t="s">
         <v>121</v>
       </c>
       <c r="I78" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D79" t="s">
+        <v>124</v>
+      </c>
+      <c r="G79" t="s">
+        <v>121</v>
+      </c>
+      <c r="I79" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="81" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="D81" s="24" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="82" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="D82" t="s">
+        <v>126</v>
+      </c>
+      <c r="G82" t="s">
+        <v>125</v>
+      </c>
+      <c r="I82" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="83" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="D83" t="s">
         <v>122</v>
       </c>
-      <c r="G79" t="s">
-        <v>131</v>
-      </c>
-      <c r="I79" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="80" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D80" t="s">
-        <v>123</v>
-      </c>
-      <c r="G80" t="s">
-        <v>121</v>
-      </c>
-      <c r="I80" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="81" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="D81" t="s">
-        <v>124</v>
-      </c>
-      <c r="G81" t="s">
-        <v>121</v>
-      </c>
-      <c r="I81" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="83" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="D83" s="24" t="s">
+      <c r="G83" t="s">
         <v>125</v>
+      </c>
+      <c r="I83" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="84" spans="3:9" x14ac:dyDescent="0.3">
       <c r="D84" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="G84" t="s">
         <v>125</v>
       </c>
       <c r="I84" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="85" spans="3:9" x14ac:dyDescent="0.3">
       <c r="D85" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="G85" t="s">
         <v>125</v>
       </c>
       <c r="I85" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="86" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="D86" t="s">
-        <v>123</v>
-      </c>
-      <c r="G86" t="s">
-        <v>125</v>
-      </c>
-      <c r="I86" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="87" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="D87" t="s">
-        <v>127</v>
-      </c>
-      <c r="G87" t="s">
-        <v>125</v>
-      </c>
-      <c r="I87" t="s">
-        <v>143</v>
+      <c r="D87" s="24" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="88" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="D88" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="89" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="D89" s="24" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="90" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="D90" t="s">
-        <v>129</v>
+      <c r="D89" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="91" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="D91" t="s">
-        <v>130</v>
+      <c r="C91" s="29" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="92" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="D92" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="93" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C93" s="29" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="94" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="D94" t="s">
-        <v>134</v>
+      <c r="D93" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="95" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="D95" t="s">
-        <v>133</v>
+      <c r="C95" s="29" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="96" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="D96" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="97" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C97" s="29" t="s">
-        <v>144</v>
+      <c r="D97" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="98" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D98" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="99" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="D99" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="100" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="D100" t="s">
-        <v>147</v>
+      <c r="C100" s="29" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="101" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D101" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="102" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C102" s="29" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="103" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="D103" t="s">
-        <v>150</v>
+      <c r="D102" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="104" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="D104" t="s">
-        <v>149</v>
+      <c r="C104" s="29" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="105" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D105" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="106" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C106" s="29" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="107" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="D107" t="s">
-        <v>151</v>
+      <c r="D106" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="108" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="D108" t="s">
-        <v>152</v>
+      <c r="C108" s="29" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="109" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D109" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="110" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C110" s="29" t="s">
-        <v>153</v>
+      <c r="D110" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="111" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D111" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="112" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D112" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="113" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D113" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="114" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D114" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="115" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D115" t="s">
         <v>158</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add lo-Fi prototype for home page
</commit_message>
<xml_diff>
--- a/3402 Ass2.xlsx
+++ b/3402 Ass2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\16567\Documents\GitHub\2023_SP51_CMS_GroupB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A1A8961-2829-457D-8684-3BB684B878CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E233C76-D8F5-475F-BD78-D2B76DCDF04A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3040" yWindow="2750" windowWidth="14190" windowHeight="11650" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks Description" sheetId="1" r:id="rId1"/>
@@ -2087,8 +2087,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EAC2AC4-0C1C-43C2-BF40-AC3F49B518A9}">
   <dimension ref="B2:J113"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P88" sqref="P88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>

</xml_diff>